<commit_message>
Adding classes for markets to customize the prices retrieval
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="338">
   <si>
     <t xml:space="preserve">JAÚ SERVE</t>
   </si>
@@ -876,6 +876,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=5601252231164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azeite Tipo Único garrafa vidro</t>
   </si>
   <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/azeite-puro-gallo-500ml-1067</t>
@@ -3638,10 +3641,10 @@
   </sheetPr>
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3939,7 +3942,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>186</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>32</v>
@@ -3948,10 +3951,10 @@
         <v>33</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3968,7 +3971,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3976,16 +3979,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3993,16 +3996,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4019,7 +4022,7 @@
         <v>40</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4051,10 +4054,10 @@
         <v>45</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4062,7 +4065,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>47</v>
@@ -4072,7 +4075,7 @@
       </c>
       <c r="E23" s="29"/>
       <c r="F23" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4089,7 +4092,7 @@
         <v>48</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4097,7 +4100,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>47</v>
@@ -4106,10 +4109,10 @@
         <v>48</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4126,10 +4129,10 @@
         <v>10</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4137,7 +4140,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>52</v>
@@ -4146,10 +4149,10 @@
         <v>53</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4166,10 +4169,10 @@
         <v>55</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4177,16 +4180,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>32</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,7 +4197,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>32</v>
@@ -4203,7 +4206,7 @@
         <v>57</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4211,7 +4214,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>32</v>
@@ -4220,10 +4223,10 @@
         <v>59</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4234,13 +4237,13 @@
         <v>60</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>62</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4257,7 +4260,7 @@
         <v>62</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4274,7 +4277,7 @@
         <v>62</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,19 +4285,19 @@
         <v>33</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>66</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4305,16 +4308,16 @@
         <v>68</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>70</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,7 +4325,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>44</v>
@@ -4331,7 +4334,7 @@
         <v>72</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4348,10 +4351,10 @@
         <v>72</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4368,10 +4371,10 @@
         <v>75</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4388,10 +4391,10 @@
         <v>62</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4399,7 +4402,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>77</v>
@@ -4409,7 +4412,7 @@
       </c>
       <c r="E41" s="29"/>
       <c r="F41" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4426,10 +4429,10 @@
         <v>62</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,10 +4449,10 @@
         <v>62</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4466,7 +4469,7 @@
         <v>84</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4483,10 +4486,10 @@
         <v>87</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4503,7 +4506,7 @@
         <v>89</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4514,13 +4517,13 @@
         <v>90</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>92</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4528,19 +4531,19 @@
         <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>91</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4548,7 +4551,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>94</v>
@@ -4557,7 +4560,7 @@
         <v>95</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4565,7 +4568,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>94</v>
@@ -4574,7 +4577,7 @@
         <v>95</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4591,10 +4594,10 @@
         <v>97</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4602,7 +4605,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>99</v>
@@ -4611,7 +4614,7 @@
         <v>100</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,7 +4622,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>99</v>
@@ -4628,10 +4631,10 @@
         <v>101</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4648,10 +4651,10 @@
         <v>104</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4668,10 +4671,10 @@
         <v>106</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4679,7 +4682,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>91</v>
@@ -4689,7 +4692,7 @@
       </c>
       <c r="E56" s="29"/>
       <c r="F56" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4706,10 +4709,10 @@
         <v>108</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4726,10 +4729,10 @@
         <v>106</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4737,7 +4740,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>16</v>
@@ -4746,7 +4749,7 @@
         <v>111</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4754,7 +4757,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>32</v>
@@ -4763,7 +4766,7 @@
         <v>42</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4771,7 +4774,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>32</v>
@@ -4780,7 +4783,7 @@
         <v>42</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,10 +4800,10 @@
         <v>114</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4817,10 +4820,10 @@
         <v>114</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4828,19 +4831,19 @@
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4857,10 +4860,10 @@
         <v>117</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4877,10 +4880,10 @@
         <v>108</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4912,10 +4915,10 @@
         <v>122</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4923,7 +4926,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>69</v>
@@ -4932,10 +4935,10 @@
         <v>48</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4943,7 +4946,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>69</v>
@@ -4952,10 +4955,10 @@
         <v>124</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4963,19 +4966,19 @@
         <v>69</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E71" s="29" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4992,10 +4995,10 @@
         <v>127</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5009,10 +5012,10 @@
         <v>126</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E73" s="29" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5020,7 +5023,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>81</v>
@@ -5029,10 +5032,10 @@
         <v>130</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5049,7 +5052,7 @@
         <v>130</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5057,7 +5060,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>132</v>
@@ -5066,7 +5069,7 @@
         <v>133</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5074,7 +5077,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>132</v>
@@ -5083,7 +5086,7 @@
         <v>133</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5100,10 +5103,10 @@
         <v>137</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5120,10 +5123,10 @@
         <v>21</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5140,7 +5143,7 @@
         <v>137</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5157,7 +5160,7 @@
         <v>21</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5174,7 +5177,7 @@
         <v>139</v>
       </c>
       <c r="E82" s="29" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5191,7 +5194,7 @@
         <v>139</v>
       </c>
       <c r="E83" s="29" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5199,16 +5202,16 @@
         <v>82</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>142</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5225,10 +5228,10 @@
         <v>30</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,10 +5248,10 @@
         <v>147</v>
       </c>
       <c r="E86" s="29" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5265,7 +5268,7 @@
         <v>148</v>
       </c>
       <c r="E87" s="29" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5282,10 +5285,10 @@
         <v>149</v>
       </c>
       <c r="E88" s="29" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F88" s="30" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5302,10 +5305,10 @@
         <v>152</v>
       </c>
       <c r="E89" s="29" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5322,10 +5325,10 @@
         <v>155</v>
       </c>
       <c r="E90" s="29" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adding option to output the result to excel file
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="374">
   <si>
     <t xml:space="preserve">JAÚ SERVE</t>
   </si>
@@ -812,6 +812,9 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/acucar-cristal-organico-uniao-1kg-12562</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891910020034</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/agua-sanitaria-super-candida-2l-1278</t>
   </si>
   <si>
@@ -851,6 +854,9 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-integral-camil-1kg-1647</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7896006755517</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/atum-ralado-ao-natural-gomes-da-costa-170g-5873</t>
   </si>
   <si>
@@ -899,6 +905,9 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/biscoito-sabor-leite-e-aveia-belvita-75g-16371</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7622210661746</t>
+  </si>
+  <si>
     <t xml:space="preserve">225g</t>
   </si>
   <si>
@@ -908,6 +917,15 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/bisnaguinha-panco-300g-568</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891203010605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branqueador banheiro sem cloro Squeeze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891035000058</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/cafe-tradicional-pilao-500g-244</t>
   </si>
   <si>
@@ -968,6 +986,12 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/limpador-sanitario-cloro-gel-ativo-marine-pato-500ml-27154</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7894650013472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7894650182208</t>
+  </si>
+  <si>
     <t xml:space="preserve">Detergente Líquido Neutro</t>
   </si>
   <si>
@@ -986,9 +1010,21 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/embalagem-multiuso-para-freezer-wyda-3kg-17535</t>
   </si>
   <si>
+    <t xml:space="preserve">100 unidades (3kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7898930672649&amp;ajax=true</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/embalagem-multiuso-para-freezer-wyda-5kg-17539</t>
   </si>
   <si>
+    <t xml:space="preserve">100 unidades (5kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7898930672656</t>
+  </si>
+  <si>
     <t xml:space="preserve">Esponja Multiuso</t>
   </si>
   <si>
@@ -1016,6 +1052,9 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/farinha-kimilho-flocao-yoki-500g-1712</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891095006878</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/farofa-pronta-de-mandioca-yoki-500g-629</t>
   </si>
   <si>
@@ -1061,6 +1100,12 @@
     <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891022101003</t>
   </si>
   <si>
+    <t xml:space="preserve">1,2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7500435115827</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/lava-roupa-liq-ariel-conc-t-downy-2l-15238</t>
   </si>
   <si>
@@ -1094,12 +1139,24 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/mistura-lactea-condensada-mococa-lata-395g</t>
   </si>
   <si>
+    <t xml:space="preserve">Leite Condensado semi desnatado caixa</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/leite-condensado-semidesnatado-italac-395g-2059</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7898080640413</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7898215152002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leite Condensado zero lactose caixa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7898215151999</t>
+  </si>
+  <si>
     <t xml:space="preserve">Leite de coco em vidro</t>
   </si>
   <si>
@@ -1154,6 +1211,9 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/limpador-veja-x14-banheiro-squeeze-500ml-6524</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891035209505</t>
+  </si>
+  <si>
     <t xml:space="preserve">Limpeza X14 Squeeze 2x1</t>
   </si>
   <si>
@@ -1196,6 +1256,12 @@
     <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7898215151425</t>
   </si>
   <si>
+    <t xml:space="preserve">Milho p/ canjica branco Tipo 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891095100293</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/milho-verde-quero-170g-30981</t>
   </si>
   <si>
@@ -1244,6 +1310,12 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/oleo-de-girassol-soya-900ml-20073</t>
   </si>
   <si>
+    <t xml:space="preserve">Pão de forma integral pacote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891203063311</t>
+  </si>
+  <si>
     <t xml:space="preserve">Papel Higiênico Folha Dupla 30m</t>
   </si>
   <si>
@@ -1253,6 +1325,9 @@
     <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7896018704275</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7896018704282</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/papel-higienico-folha-tripla-neve-20m-leve-24-pague-21-rolos-29414</t>
   </si>
   <si>
@@ -1262,12 +1337,39 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/creme-dental-tripla-acao-hortela-colgate-90g</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891024132128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasta dental Sensitive Pro-Alívio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891024123560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891024132647</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pasta dental Sensitive Pro-Alívio Imediato</t>
   </si>
   <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/creme-dental-sensitive-pro-alivio-colgate-90g-28079</t>
   </si>
   <si>
+    <t xml:space="preserve">Requeijão cremoso tradicional copo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vigor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891999144485</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-pedra-urca-coco-5-unidades-200g-11265</t>
   </si>
   <si>
@@ -1283,6 +1385,9 @@
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-pedra-urca-coco-premium-200g-11296</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7896056401983</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-de-pedra-de-coco-ype-200g-27172</t>
   </si>
   <si>
@@ -1299,6 +1404,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/sal-refinado-cisne-1kg-304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7896035210001</t>
   </si>
   <si>
     <t xml:space="preserve">https://tenda-api.stoomlab.com.br/api/public/store/product/sardinha-em-oleo-gomes-da-costa-125g-525</t>
@@ -1344,7 +1452,7 @@
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1420,6 +1528,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1500,7 +1614,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1641,6 +1755,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1726,7 +1844,7 @@
       <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -3589,7 +3707,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.14"/>
   </cols>
@@ -3622,7 +3740,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3639,15 +3757,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.74"/>
@@ -3742,6 +3860,9 @@
       <c r="E5" s="29" t="s">
         <v>163</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="n">
@@ -3757,7 +3878,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,10 +3895,10 @@
         <v>21</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3794,10 +3915,10 @@
         <v>24</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,10 +3935,10 @@
         <v>27</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,10 +3955,10 @@
         <v>27</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3845,7 +3966,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>12</v>
@@ -3854,10 +3975,10 @@
         <v>27</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,7 +3986,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>12</v>
@@ -3874,7 +3995,10 @@
         <v>75</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>176</v>
+        <v>177</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,10 +4015,10 @@
         <v>30</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3902,19 +4026,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,10 +4055,10 @@
         <v>33</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3942,7 +4066,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>32</v>
@@ -3951,10 +4075,10 @@
         <v>33</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3971,7 +4095,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3979,16 +4103,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>192</v>
+        <v>194</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3996,16 +4123,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="D19" s="32" t="s">
-        <v>191</v>
-      </c>
       <c r="E19" s="29" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4022,7 +4149,10 @@
         <v>40</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>195</v>
+        <v>198</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4030,7 +4160,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>32</v>
@@ -4039,6 +4169,9 @@
         <v>42</v>
       </c>
       <c r="E21" s="33"/>
+      <c r="F21" s="0" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="n">
@@ -4054,10 +4187,10 @@
         <v>45</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4065,7 +4198,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>47</v>
@@ -4075,7 +4208,7 @@
       </c>
       <c r="E23" s="29"/>
       <c r="F23" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4092,7 +4225,7 @@
         <v>48</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,7 +4233,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>47</v>
@@ -4109,10 +4242,10 @@
         <v>48</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4129,10 +4262,10 @@
         <v>10</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4140,7 +4273,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>52</v>
@@ -4149,10 +4282,10 @@
         <v>53</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4169,10 +4302,10 @@
         <v>55</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4180,16 +4313,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>32</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4197,7 +4330,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>32</v>
@@ -4206,7 +4339,10 @@
         <v>57</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>215</v>
+        <v>221</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4214,19 +4350,17 @@
         <v>29</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>32</v>
+        <v>154</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>217</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E31" s="29"/>
       <c r="F31" s="0" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4234,16 +4368,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>219</v>
+        <v>32</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>220</v>
+        <v>225</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,13 +4391,13 @@
         <v>60</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>61</v>
+        <v>227</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>62</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4268,1255 +4405,1478 @@
         <v>32</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>62</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="28" t="n">
-        <v>33</v>
-      </c>
+      <c r="A35" s="28"/>
       <c r="B35" s="10" t="s">
-        <v>223</v>
+        <v>60</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>66</v>
+        <v>230</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>225</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E35" s="29"/>
       <c r="F35" s="0" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>227</v>
+        <v>64</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="28" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>231</v>
+      <c r="A37" s="28"/>
+      <c r="B37" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="29"/>
+      <c r="F37" s="0" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>72</v>
+        <v>34</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>236</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>75</v>
+        <v>35</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>77</v>
+        <v>242</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" s="29"/>
+        <v>72</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>245</v>
+      </c>
       <c r="F41" s="0" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="28" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>83</v>
+        <v>251</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>244</v>
+        <v>62</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="0" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>247</v>
+        <v>255</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>248</v>
+        <v>83</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="28" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>250</v>
+        <v>85</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>251</v>
+        <v>87</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="28" t="n">
-        <v>47</v>
-      </c>
+      <c r="A49" s="28"/>
       <c r="B49" s="4" t="s">
-        <v>254</v>
+        <v>88</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>94</v>
+        <v>260</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E49" s="29" t="s">
-        <v>255</v>
+        <v>89</v>
+      </c>
+      <c r="E49" s="29"/>
+      <c r="F49" s="0" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>256</v>
+        <v>88</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>94</v>
+        <v>263</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="28" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>260</v>
+        <v>47</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>265</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>100</v>
+        <v>266</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>261</v>
+        <v>267</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" s="24" t="s">
-        <v>260</v>
+        <v>48</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>269</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="28" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>102</v>
+        <v>271</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="28" t="n">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>105</v>
+        <v>273</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="28" t="n">
-        <v>54</v>
-      </c>
+      <c r="A56" s="28"/>
       <c r="B56" s="4" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E56" s="29"/>
       <c r="F56" s="0" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="28" t="n">
-        <v>55</v>
-      </c>
+      <c r="A57" s="28"/>
       <c r="B57" s="4" t="s">
-        <v>107</v>
+        <v>277</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="29" t="s">
-        <v>270</v>
-      </c>
+      <c r="E57" s="29"/>
       <c r="F57" s="0" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>109</v>
+        <v>51</v>
+      </c>
+      <c r="B58" s="24" t="s">
+        <v>279</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="F58" s="0" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>274</v>
+        <v>52</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>279</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>275</v>
+        <v>281</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>276</v>
+        <v>102</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>277</v>
+        <v>283</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>278</v>
+        <v>105</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>279</v>
+        <v>285</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C62" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D62" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>280</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E62" s="29"/>
       <c r="F62" s="0" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="n">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="n">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>284</v>
+        <v>109</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>285</v>
+        <v>91</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>116</v>
+        <v>293</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>288</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>118</v>
+        <v>295</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>119</v>
+        <v>298</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E67" s="33"/>
+        <v>42</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28" t="n">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>122</v>
+        <v>113</v>
+      </c>
+      <c r="C68" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" s="24" t="s">
-        <v>294</v>
+        <v>62</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" s="24" t="s">
-        <v>294</v>
+        <v>63</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>304</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>69</v>
+        <v>305</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" s="34" t="s">
-        <v>299</v>
+        <v>64</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>300</v>
+        <v>36</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>301</v>
+        <v>117</v>
       </c>
       <c r="E71" s="29" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" s="24" t="s">
-        <v>125</v>
+        <v>65</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" s="24" t="s">
-        <v>125</v>
+        <v>66</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="E73" s="29" t="s">
-        <v>307</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="E73" s="33"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="28" t="n">
+      <c r="A74" s="28"/>
+      <c r="B74" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E74" s="29" t="s">
-        <v>309</v>
-      </c>
+      <c r="E74" s="33"/>
       <c r="F74" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="n">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>311</v>
+        <v>314</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>312</v>
+        <v>68</v>
+      </c>
+      <c r="B76" s="24" t="s">
+        <v>316</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>313</v>
+        <v>317</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" s="34" t="s">
-        <v>314</v>
+        <v>69</v>
+      </c>
+      <c r="B77" s="24" t="s">
+        <v>316</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>315</v>
+        <v>319</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" s="24" t="s">
-        <v>135</v>
+        <v>70</v>
+      </c>
+      <c r="B78" s="34" t="s">
+        <v>321</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>136</v>
+        <v>322</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>137</v>
+        <v>323</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="n">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="n">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>137</v>
+        <v>328</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="28" t="n">
-        <v>79</v>
-      </c>
+      <c r="A81" s="28"/>
       <c r="B81" s="24" t="s">
-        <v>135</v>
+        <v>330</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E81" s="29" t="s">
-        <v>321</v>
+        <v>40</v>
+      </c>
+      <c r="E81" s="29"/>
+      <c r="F81" s="0" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>138</v>
+        <v>332</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E82" s="29" t="s">
-        <v>322</v>
+        <v>333</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="28" t="n">
+      <c r="A83" s="28"/>
+      <c r="B83" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="D83" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E83" s="29" t="s">
-        <v>323</v>
+        <v>130</v>
+      </c>
+      <c r="E83" s="29"/>
+      <c r="F83" s="0" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="n">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>324</v>
+        <v>128</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>325</v>
+        <v>129</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="n">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>143</v>
+        <v>337</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="28" t="n">
-        <v>84</v>
-      </c>
-      <c r="B86" s="24" t="s">
-        <v>145</v>
+      <c r="A86" s="28"/>
+      <c r="B86" s="35" t="s">
+        <v>340</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>146</v>
+        <v>341</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E86" s="29" t="s">
-        <v>329</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E86" s="29"/>
       <c r="F86" s="0" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="28" t="n">
-        <v>85</v>
-      </c>
-      <c r="B87" s="24" t="s">
-        <v>145</v>
+      <c r="A87" s="28"/>
+      <c r="B87" s="35" t="s">
+        <v>340</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>146</v>
+        <v>343</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E87" s="29" t="s">
-        <v>331</v>
+        <v>133</v>
+      </c>
+      <c r="E87" s="29"/>
+      <c r="F87" s="0" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="n">
-        <v>86</v>
-      </c>
-      <c r="B88" s="24" t="s">
-        <v>145</v>
+        <v>76</v>
+      </c>
+      <c r="B88" s="34" t="s">
+        <v>345</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="E88" s="29" t="s">
-        <v>332</v>
-      </c>
-      <c r="F88" s="30" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="28" t="n">
-        <v>87</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>150</v>
+      <c r="A89" s="28"/>
+      <c r="B89" s="34" t="s">
+        <v>347</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>151</v>
+        <v>36</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E89" s="29" t="s">
-        <v>334</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="E89" s="29"/>
       <c r="F89" s="0" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="28" t="n">
+        <v>77</v>
+      </c>
+      <c r="B90" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="28" t="n">
+        <v>78</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E91" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="28" t="n">
+        <v>79</v>
+      </c>
+      <c r="B92" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="28" t="n">
+        <v>80</v>
+      </c>
+      <c r="B93" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93" s="29" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="28" t="n">
+        <v>81</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E94" s="29" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="28" t="n">
+        <v>82</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E95" s="29" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="28" t="n">
+        <v>83</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E96" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="28" t="n">
+        <v>84</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E97" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="28" t="n">
+        <v>85</v>
+      </c>
+      <c r="B98" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="28" t="n">
+        <v>86</v>
+      </c>
+      <c r="B99" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E99" s="29" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="28" t="n">
+        <v>87</v>
+      </c>
+      <c r="B100" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100" s="29" t="s">
+        <v>368</v>
+      </c>
+      <c r="F100" s="30" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="28" t="n">
         <v>88</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B101" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E101" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="28" t="n">
+        <v>89</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C102" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D102" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E90" s="29" t="s">
-        <v>336</v>
-      </c>
-      <c r="F90" s="0" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
+      <c r="E102" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C104" s="25"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C106" s="25"/>
-      <c r="D106" s="25"/>
-      <c r="E106" s="25"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="25"/>
-      <c r="D107" s="25"/>
-      <c r="E107" s="25"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C108" s="25"/>
-      <c r="D108" s="25"/>
-      <c r="E108" s="25"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C109" s="25"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="25"/>
-      <c r="D110" s="25"/>
-      <c r="E110" s="25"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C115" s="25"/>
+      <c r="D115" s="25"/>
+      <c r="E115" s="25"/>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C116" s="25"/>
+      <c r="D116" s="25"/>
+      <c r="E116" s="25"/>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C117" s="25"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="25"/>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C118" s="25"/>
+      <c r="D118" s="25"/>
+      <c r="E118" s="25"/>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C119" s="25"/>
+      <c r="D119" s="25"/>
+      <c r="E119" s="25"/>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C120" s="25"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="25"/>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C121" s="25"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="25"/>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="25"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" display="https://tenda-api.stoomlab.com.br/api/public/store/product/achocolatado-em-po-nescau-400g-2348 "/>
     <hyperlink ref="E4" r:id="rId2" display="https://tenda-api.stoomlab.com.br/api/public/store/product/acucar-refinado-uniao-1kg-60"/>
     <hyperlink ref="E5" r:id="rId3" display="https://tenda-api.stoomlab.com.br/api/public/store/product/acucar-cristal-organico-uniao-1kg-12562"/>
-    <hyperlink ref="E6" r:id="rId4" display="https://tenda-api.stoomlab.com.br/api/public/store/product/agua-sanitaria-super-candida-2l-1278"/>
-    <hyperlink ref="E7" r:id="rId5" display="https://tenda-api.stoomlab.com.br/api/public/store/product/amaciante-fleur-d-ype-aconchego-azul-2l-888"/>
-    <hyperlink ref="E8" r:id="rId6" display="https://tenda-api.stoomlab.com.br/api/public/store/product/alvejante-em-barra-super-white-vanish-75g-27490"/>
-    <hyperlink ref="E9" r:id="rId7" display="https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-tipo-1-prato-fino-1kg-2092"/>
-    <hyperlink ref="E10" r:id="rId8" display="https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-tipo-1-prato-fino-5kg-835"/>
-    <hyperlink ref="E11" r:id="rId9" display="https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-integral-prato-fino-1kg-2591"/>
-    <hyperlink ref="E12" r:id="rId10" display="https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-integral-camil-1kg-1647"/>
-    <hyperlink ref="E13" r:id="rId11" display="https://tenda-api.stoomlab.com.br/api/public/store/product/atum-ralado-ao-natural-gomes-da-costa-170g-5873"/>
-    <hyperlink ref="E14" r:id="rId12" display="https://tenda-api.stoomlab.com.br/api/public/store/product/aveia-em-flocos-finos-quaker-165g-3977"/>
-    <hyperlink ref="E15" r:id="rId13" display="https://tenda-api.stoomlab.com.br/api/public/store/product/azeite-extra-virgem-gallo-500ml-317"/>
-    <hyperlink ref="F15" r:id="rId14" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=5601252231164"/>
-    <hyperlink ref="E16" r:id="rId15" display="https://tenda-api.stoomlab.com.br/api/public/store/product/azeite-puro-gallo-500ml-1067"/>
-    <hyperlink ref="E17" r:id="rId16" display="https://tenda-api.stoomlab.com.br/api/public/store/product/azeitona-verde-com-caroco-imperador-200g"/>
-    <hyperlink ref="E18" r:id="rId17" display="https://tenda-api.stoomlab.com.br/api/public/store/product/biscoito-sabor-leite-e-aveia-belvita-75g-16371"/>
-    <hyperlink ref="E19" r:id="rId18" display="https://tenda-api.stoomlab.com.br/api/public/store/product/biscoito-sabor-leite-e-aveia-belvita-225g-16375"/>
-    <hyperlink ref="E20" r:id="rId19" display="https://tenda-api.stoomlab.com.br/api/public/store/product/bisnaguinha-panco-300g-568"/>
-    <hyperlink ref="E22" r:id="rId20" display="https://tenda-api.stoomlab.com.br/api/public/store/product/cafe-tradicional-pilao-500g-244"/>
-    <hyperlink ref="E24" r:id="rId21" display="https://tenda-api.stoomlab.com.br/api/public/store/product/ketchup-picante-heinz-397-g"/>
-    <hyperlink ref="E25" r:id="rId22" display="https://tenda-api.stoomlab.com.br/api/public/store/product/catchup-picles-heinz-397g"/>
-    <hyperlink ref="E26" r:id="rId23" display="https://tenda-api.stoomlab.com.br/api/public/store/product/cereal-matinal-nescau-nestle-270g-1608"/>
-    <hyperlink ref="F26" r:id="rId24" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891000111161"/>
-    <hyperlink ref="E27" r:id="rId25" display="https://tenda-api.stoomlab.com.br/api/public/store/product/cerveja-puro-malte-tipo-pilsen-imperio-350ml-23328"/>
-    <hyperlink ref="E28" r:id="rId26" display="https://tenda-api.stoomlab.com.br/api/public/store/product/cerveja-brahma-duplo-malte-lata-sleek-350ml"/>
-    <hyperlink ref="E29" r:id="rId27" display="https://tenda-api.stoomlab.com.br/api/public/store/product/desinfetante-lavanda-active-fresh-harpic-500ml"/>
-    <hyperlink ref="E30" r:id="rId28" display="https://tenda-api.stoomlab.com.br/api/public/store/product/limpador-sanitario-cloro-gel-ativo-marine-pato-500ml-27154"/>
-    <hyperlink ref="E31" r:id="rId29" display="https://tenda-api.stoomlab.com.br/api/public/store/product/detergente-liquido-limpol-neutro-500ml-182"/>
-    <hyperlink ref="E32" r:id="rId30" display="https://tenda-api.stoomlab.com.br/api/public/store/product/embalagem-multiuso-para-freezer-wyda-2kg-17537"/>
-    <hyperlink ref="E33" r:id="rId31" display="https://tenda-api.stoomlab.com.br/api/public/store/product/embalagem-multiuso-para-freezer-wyda-3kg-17535"/>
-    <hyperlink ref="E34" r:id="rId32" display="https://tenda-api.stoomlab.com.br/api/public/store/product/embalagem-multiuso-para-freezer-wyda-5kg-17539"/>
-    <hyperlink ref="E35" r:id="rId33" display="https://tenda-api.stoomlab.com.br/api/public/store/product/esponja-m-u-scotch-brite-6115"/>
-    <hyperlink ref="E36" r:id="rId34" display="https://tenda-api.stoomlab.com.br/api/public/store/product/ext-tom-elefante-pt-310g"/>
-    <hyperlink ref="E37" r:id="rId35" display="https://tenda-api.stoomlab.com.br/api/public/store/product/farinha-kimilho-flocao-yoki-500g-1712"/>
-    <hyperlink ref="E38" r:id="rId36" display="https://tenda-api.stoomlab.com.br/api/public/store/product/farofa-pronta-de-mandioca-yoki-500g-629"/>
-    <hyperlink ref="E39" r:id="rId37" display="https://tenda-api.stoomlab.com.br/api/public/store/product/feijao-carioca-tipo-1-camil-1kg-481"/>
-    <hyperlink ref="E40" r:id="rId38" display="https://tenda-api.stoomlab.com.br/api/public/store/product/filme-pvc-30-25-wyda-28cmx30m-626"/>
-    <hyperlink ref="E42" r:id="rId39" display="https://tenda-api.stoomlab.com.br/api/public/store/product/folha-de-aluminio-r45-7-5m-wyda-592"/>
-    <hyperlink ref="E43" r:id="rId40" display="https://tenda-api.stoomlab.com.br/api/public/store/product/forro-para-fogao-wyda-12un-16650"/>
-    <hyperlink ref="E44" r:id="rId41" display="https://tenda-api.stoomlab.com.br/api/public/store/product/haste-flex-topz-300un--14215"/>
-    <hyperlink ref="E45" r:id="rId42" display="https://tenda-api.stoomlab.com.br/api/public/store/product/la-de-aco-bombril-8un-130"/>
-    <hyperlink ref="E46" r:id="rId43" display="https://tenda-api.stoomlab.com.br/api/public/store/product/lava-roupa-liq-ariel-conc-t-downy-2l-15238"/>
-    <hyperlink ref="E47" r:id="rId44" display="https://tenda-api.stoomlab.com.br/api/public/store/product/lava-roupa-liquido-ares-5l-13943"/>
-    <hyperlink ref="E48" r:id="rId45" display="https://tenda-api.stoomlab.com.br/api/public/store/product/lava-roupa-liquido-ola-coco-1l-11470"/>
-    <hyperlink ref="E49" r:id="rId46" display="https://tenda-api.stoomlab.com.br/api/public/store/product/mistura-lactea-condensada-mococa-caixa-395g-30254"/>
-    <hyperlink ref="E50" r:id="rId47" display="https://tenda-api.stoomlab.com.br/api/public/store/product/mistura-lactea-condensada-mococa-lata-395g"/>
-    <hyperlink ref="E51" r:id="rId48" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-condensado-semidesnatado-italac-395g-2059"/>
-    <hyperlink ref="E52" r:id="rId49" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-de-coco-menina-200ml-1144"/>
-    <hyperlink ref="E53" r:id="rId50" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-de-coco-sococo-200ml-227"/>
-    <hyperlink ref="E54" r:id="rId51" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-em-po-desnatado-molico-280g-7412"/>
-    <hyperlink ref="E55" r:id="rId52" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-longa-vida-zero-lactose-ninho-1l-23532"/>
-    <hyperlink ref="E57" r:id="rId53" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-semi-desnatado-piracanjuba-zero-lactose-1l-7642"/>
-    <hyperlink ref="E58" r:id="rId54" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-longa-vida-semidesnatado-levinho-ninho-1l-20130"/>
-    <hyperlink ref="E59" r:id="rId55" display="https://tenda-api.stoomlab.com.br/api/public/store/product/limpador-perfumado-sensualidade-casa-e-perfume-2l-7162"/>
-    <hyperlink ref="E60" r:id="rId56" display="https://tenda-api.stoomlab.com.br/api/public/store/product/limpador-veja-x14-banheiro-squeeze-500ml-6524"/>
-    <hyperlink ref="E62" r:id="rId57" display="https://tenda-api.stoomlab.com.br/api/public/store/product/macarrao-com-ovos-barilla-penne-500g-7203"/>
-    <hyperlink ref="E63" r:id="rId58" display="https://tenda-api.stoomlab.com.br/api/public/store/product/macarrao-grano-duro-barilla-spaghettini-3-500g-6353"/>
-    <hyperlink ref="E64" r:id="rId59" display="https://tenda-api.stoomlab.com.br/api/public/store/product/maionese-heinz-pet-390g-8979"/>
-    <hyperlink ref="E65" r:id="rId60" display="https://tenda-api.stoomlab.com.br/api/public/store/product/manteiga-aviacao-pote-com-sal-200g-1030"/>
-    <hyperlink ref="E66" r:id="rId61" display="https://tenda-api.stoomlab.com.br/api/public/store/product/manteiga-com-sal-zero-lactose-piracanjuba-200g-32822"/>
-    <hyperlink ref="E68" r:id="rId62" display="https://tenda-api.stoomlab.com.br/api/public/store/product/milho-verde-quero-170g-30981"/>
-    <hyperlink ref="E69" r:id="rId63" display="https://tenda-api.stoomlab.com.br/api/public/store/product/molho-trad-heinz-sache-340g-9067"/>
-    <hyperlink ref="E70" r:id="rId64" display="https://tenda-api.stoomlab.com.br/api/public/store/product/molho-de-tomate-tradicional-refogado-pomarola-sache-340g-2484"/>
-    <hyperlink ref="E71" r:id="rId65" display="https://tenda-api.stoomlab.com.br/api/public/store/product/purificador-de-ar-click-spray-cheirinho-de-limpeza-bom-ar-refil-12ml-leve-3-pague-2-27508"/>
-    <hyperlink ref="E72" r:id="rId66" display="https://tenda-api.stoomlab.com.br/api/public/store/product/oleo-de-girassol-liza-pet-900ml-878"/>
-    <hyperlink ref="E73" r:id="rId67" display="https://tenda-api.stoomlab.com.br/api/public/store/product/oleo-de-girassol-soya-900ml-20073"/>
-    <hyperlink ref="E74" r:id="rId68" display="https://tenda-api.stoomlab.com.br/api/public/store/product/papel-higienico-folha-dupla-toque-da-seda-30m-neve-leve-12-pague-11"/>
-    <hyperlink ref="E75" r:id="rId69" display="https://tenda-api.stoomlab.com.br/api/public/store/product/papel-higienico-folha-tripla-neve-20m-leve-24-pague-21-rolos-29414"/>
-    <hyperlink ref="E76" r:id="rId70" display="https://tenda-api.stoomlab.com.br/api/public/store/product/creme-dental-tripla-acao-hortela-colgate-90g"/>
-    <hyperlink ref="E77" r:id="rId71" display="https://tenda-api.stoomlab.com.br/api/public/store/product/creme-dental-sensitive-pro-alivio-colgate-90g-28079"/>
-    <hyperlink ref="E78" r:id="rId72" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-pedra-urca-coco-5-unidades-200g-11265"/>
-    <hyperlink ref="E79" r:id="rId73" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-em-pedra-ype-coco-5x200g-4199"/>
-    <hyperlink ref="E80" r:id="rId74" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-pedra-urca-coco-premium-200g-11296"/>
-    <hyperlink ref="E81" r:id="rId75" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-de-pedra-de-coco-ype-200g-27172"/>
-    <hyperlink ref="E82" r:id="rId76" display="https://tenda-api.stoomlab.com.br/api/public/store/product/refil-sabonete-liquido-buque-de-jasmim-lux-220ml-24428"/>
-    <hyperlink ref="E83" r:id="rId77" display="https://tenda-api.stoomlab.com.br/api/public/store/product/refil-sabonete-liquido-flor-de-lotus-lux-200ml-24434"/>
-    <hyperlink ref="E84" r:id="rId78" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sal-refinado-cisne-1kg-304"/>
-    <hyperlink ref="E85" r:id="rId79" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sardinha-em-oleo-gomes-da-costa-125g-525"/>
-    <hyperlink ref="E86" r:id="rId80" display="https://tenda-api.stoomlab.com.br/api/public/store/product/papel-toalha-kitchen-2-unidades-1232"/>
-    <hyperlink ref="E87" r:id="rId81" display="https://tenda-api.stoomlab.com.br/api/public/store/product/toalha-papel-snack-2un-19510"/>
-    <hyperlink ref="E88" r:id="rId82" display="https://tenda-api.stoomlab.com.br/api/public/store/product/papel-toalha-snob-neutro-2-unidades-3291"/>
-    <hyperlink ref="E89" r:id="rId83" display="https://tenda-api.stoomlab.com.br/api/public/store/product/torrada-integral-bauducco-284g-27962"/>
-    <hyperlink ref="E90" r:id="rId84" display="https://tenda-api.stoomlab.com.br/api/public/store/product/vinagre-de-fruta-castelo-maca-750ml-701"/>
+    <hyperlink ref="F5" r:id="rId4" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891910020034"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://tenda-api.stoomlab.com.br/api/public/store/product/agua-sanitaria-super-candida-2l-1278"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://tenda-api.stoomlab.com.br/api/public/store/product/amaciante-fleur-d-ype-aconchego-azul-2l-888"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://tenda-api.stoomlab.com.br/api/public/store/product/alvejante-em-barra-super-white-vanish-75g-27490"/>
+    <hyperlink ref="E9" r:id="rId8" display="https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-tipo-1-prato-fino-1kg-2092"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-tipo-1-prato-fino-5kg-835"/>
+    <hyperlink ref="E11" r:id="rId10" display="https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-integral-prato-fino-1kg-2591"/>
+    <hyperlink ref="E12" r:id="rId11" display="https://tenda-api.stoomlab.com.br/api/public/store/product/arroz-integral-camil-1kg-1647"/>
+    <hyperlink ref="F12" r:id="rId12" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7896006755517"/>
+    <hyperlink ref="E13" r:id="rId13" display="https://tenda-api.stoomlab.com.br/api/public/store/product/atum-ralado-ao-natural-gomes-da-costa-170g-5873"/>
+    <hyperlink ref="E14" r:id="rId14" display="https://tenda-api.stoomlab.com.br/api/public/store/product/aveia-em-flocos-finos-quaker-165g-3977"/>
+    <hyperlink ref="E15" r:id="rId15" display="https://tenda-api.stoomlab.com.br/api/public/store/product/azeite-extra-virgem-gallo-500ml-317"/>
+    <hyperlink ref="F15" r:id="rId16" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=5601252231164"/>
+    <hyperlink ref="E16" r:id="rId17" display="https://tenda-api.stoomlab.com.br/api/public/store/product/azeite-puro-gallo-500ml-1067"/>
+    <hyperlink ref="E17" r:id="rId18" display="https://tenda-api.stoomlab.com.br/api/public/store/product/azeitona-verde-com-caroco-imperador-200g"/>
+    <hyperlink ref="E18" r:id="rId19" display="https://tenda-api.stoomlab.com.br/api/public/store/product/biscoito-sabor-leite-e-aveia-belvita-75g-16371"/>
+    <hyperlink ref="F18" r:id="rId20" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7622210661746"/>
+    <hyperlink ref="E19" r:id="rId21" display="https://tenda-api.stoomlab.com.br/api/public/store/product/biscoito-sabor-leite-e-aveia-belvita-225g-16375"/>
+    <hyperlink ref="E20" r:id="rId22" display="https://tenda-api.stoomlab.com.br/api/public/store/product/bisnaguinha-panco-300g-568"/>
+    <hyperlink ref="F20" r:id="rId23" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891203010605"/>
+    <hyperlink ref="F21" r:id="rId24" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891035000058"/>
+    <hyperlink ref="E22" r:id="rId25" display="https://tenda-api.stoomlab.com.br/api/public/store/product/cafe-tradicional-pilao-500g-244"/>
+    <hyperlink ref="E24" r:id="rId26" display="https://tenda-api.stoomlab.com.br/api/public/store/product/ketchup-picante-heinz-397-g"/>
+    <hyperlink ref="E25" r:id="rId27" display="https://tenda-api.stoomlab.com.br/api/public/store/product/catchup-picles-heinz-397g"/>
+    <hyperlink ref="E26" r:id="rId28" display="https://tenda-api.stoomlab.com.br/api/public/store/product/cereal-matinal-nescau-nestle-270g-1608"/>
+    <hyperlink ref="F26" r:id="rId29" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891000111161"/>
+    <hyperlink ref="E27" r:id="rId30" display="https://tenda-api.stoomlab.com.br/api/public/store/product/cerveja-puro-malte-tipo-pilsen-imperio-350ml-23328"/>
+    <hyperlink ref="E28" r:id="rId31" display="https://tenda-api.stoomlab.com.br/api/public/store/product/cerveja-brahma-duplo-malte-lata-sleek-350ml"/>
+    <hyperlink ref="E29" r:id="rId32" display="https://tenda-api.stoomlab.com.br/api/public/store/product/desinfetante-lavanda-active-fresh-harpic-500ml"/>
+    <hyperlink ref="E30" r:id="rId33" display="https://tenda-api.stoomlab.com.br/api/public/store/product/limpador-sanitario-cloro-gel-ativo-marine-pato-500ml-27154"/>
+    <hyperlink ref="F30" r:id="rId34" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7894650013472"/>
+    <hyperlink ref="F31" r:id="rId35" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7894650182208"/>
+    <hyperlink ref="E32" r:id="rId36" display="https://tenda-api.stoomlab.com.br/api/public/store/product/detergente-liquido-limpol-neutro-500ml-182"/>
+    <hyperlink ref="E33" r:id="rId37" display="https://tenda-api.stoomlab.com.br/api/public/store/product/embalagem-multiuso-para-freezer-wyda-2kg-17537"/>
+    <hyperlink ref="E34" r:id="rId38" display="https://tenda-api.stoomlab.com.br/api/public/store/product/embalagem-multiuso-para-freezer-wyda-3kg-17535"/>
+    <hyperlink ref="F35" r:id="rId39" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7898930672649&amp;ajax=true"/>
+    <hyperlink ref="E36" r:id="rId40" display="https://tenda-api.stoomlab.com.br/api/public/store/product/embalagem-multiuso-para-freezer-wyda-5kg-17539"/>
+    <hyperlink ref="F37" r:id="rId41" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7898930672656"/>
+    <hyperlink ref="E38" r:id="rId42" display="https://tenda-api.stoomlab.com.br/api/public/store/product/esponja-m-u-scotch-brite-6115"/>
+    <hyperlink ref="E39" r:id="rId43" display="https://tenda-api.stoomlab.com.br/api/public/store/product/ext-tom-elefante-pt-310g"/>
+    <hyperlink ref="E40" r:id="rId44" display="https://tenda-api.stoomlab.com.br/api/public/store/product/farinha-kimilho-flocao-yoki-500g-1712"/>
+    <hyperlink ref="F40" r:id="rId45" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891095006878"/>
+    <hyperlink ref="E41" r:id="rId46" display="https://tenda-api.stoomlab.com.br/api/public/store/product/farofa-pronta-de-mandioca-yoki-500g-629"/>
+    <hyperlink ref="E42" r:id="rId47" display="https://tenda-api.stoomlab.com.br/api/public/store/product/feijao-carioca-tipo-1-camil-1kg-481"/>
+    <hyperlink ref="E43" r:id="rId48" display="https://tenda-api.stoomlab.com.br/api/public/store/product/filme-pvc-30-25-wyda-28cmx30m-626"/>
+    <hyperlink ref="E45" r:id="rId49" display="https://tenda-api.stoomlab.com.br/api/public/store/product/folha-de-aluminio-r45-7-5m-wyda-592"/>
+    <hyperlink ref="E46" r:id="rId50" display="https://tenda-api.stoomlab.com.br/api/public/store/product/forro-para-fogao-wyda-12un-16650"/>
+    <hyperlink ref="E47" r:id="rId51" display="https://tenda-api.stoomlab.com.br/api/public/store/product/haste-flex-topz-300un--14215"/>
+    <hyperlink ref="E48" r:id="rId52" display="https://tenda-api.stoomlab.com.br/api/public/store/product/la-de-aco-bombril-8un-130"/>
+    <hyperlink ref="F49" r:id="rId53" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7500435115827"/>
+    <hyperlink ref="E50" r:id="rId54" display="https://tenda-api.stoomlab.com.br/api/public/store/product/lava-roupa-liq-ariel-conc-t-downy-2l-15238"/>
+    <hyperlink ref="E51" r:id="rId55" display="https://tenda-api.stoomlab.com.br/api/public/store/product/lava-roupa-liquido-ares-5l-13943"/>
+    <hyperlink ref="E52" r:id="rId56" display="https://tenda-api.stoomlab.com.br/api/public/store/product/lava-roupa-liquido-ola-coco-1l-11470"/>
+    <hyperlink ref="E53" r:id="rId57" display="https://tenda-api.stoomlab.com.br/api/public/store/product/mistura-lactea-condensada-mococa-caixa-395g-30254"/>
+    <hyperlink ref="E54" r:id="rId58" display="https://tenda-api.stoomlab.com.br/api/public/store/product/mistura-lactea-condensada-mococa-lata-395g"/>
+    <hyperlink ref="E55" r:id="rId59" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-condensado-semidesnatado-italac-395g-2059"/>
+    <hyperlink ref="E58" r:id="rId60" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-de-coco-menina-200ml-1144"/>
+    <hyperlink ref="E59" r:id="rId61" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-de-coco-sococo-200ml-227"/>
+    <hyperlink ref="E60" r:id="rId62" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-em-po-desnatado-molico-280g-7412"/>
+    <hyperlink ref="E61" r:id="rId63" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-longa-vida-zero-lactose-ninho-1l-23532"/>
+    <hyperlink ref="E63" r:id="rId64" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-semi-desnatado-piracanjuba-zero-lactose-1l-7642"/>
+    <hyperlink ref="E64" r:id="rId65" display="https://tenda-api.stoomlab.com.br/api/public/store/product/leite-longa-vida-semidesnatado-levinho-ninho-1l-20130"/>
+    <hyperlink ref="E65" r:id="rId66" display="https://tenda-api.stoomlab.com.br/api/public/store/product/limpador-perfumado-sensualidade-casa-e-perfume-2l-7162"/>
+    <hyperlink ref="E66" r:id="rId67" display="https://tenda-api.stoomlab.com.br/api/public/store/product/limpador-veja-x14-banheiro-squeeze-500ml-6524"/>
+    <hyperlink ref="E68" r:id="rId68" display="https://tenda-api.stoomlab.com.br/api/public/store/product/macarrao-com-ovos-barilla-penne-500g-7203"/>
+    <hyperlink ref="E69" r:id="rId69" display="https://tenda-api.stoomlab.com.br/api/public/store/product/macarrao-grano-duro-barilla-spaghettini-3-500g-6353"/>
+    <hyperlink ref="E70" r:id="rId70" display="https://tenda-api.stoomlab.com.br/api/public/store/product/maionese-heinz-pet-390g-8979"/>
+    <hyperlink ref="E71" r:id="rId71" display="https://tenda-api.stoomlab.com.br/api/public/store/product/manteiga-aviacao-pote-com-sal-200g-1030"/>
+    <hyperlink ref="E72" r:id="rId72" display="https://tenda-api.stoomlab.com.br/api/public/store/product/manteiga-com-sal-zero-lactose-piracanjuba-200g-32822"/>
+    <hyperlink ref="E75" r:id="rId73" display="https://tenda-api.stoomlab.com.br/api/public/store/product/milho-verde-quero-170g-30981"/>
+    <hyperlink ref="E76" r:id="rId74" display="https://tenda-api.stoomlab.com.br/api/public/store/product/molho-trad-heinz-sache-340g-9067"/>
+    <hyperlink ref="E77" r:id="rId75" display="https://tenda-api.stoomlab.com.br/api/public/store/product/molho-de-tomate-tradicional-refogado-pomarola-sache-340g-2484"/>
+    <hyperlink ref="E78" r:id="rId76" display="https://tenda-api.stoomlab.com.br/api/public/store/product/purificador-de-ar-click-spray-cheirinho-de-limpeza-bom-ar-refil-12ml-leve-3-pague-2-27508"/>
+    <hyperlink ref="E79" r:id="rId77" display="https://tenda-api.stoomlab.com.br/api/public/store/product/oleo-de-girassol-liza-pet-900ml-878"/>
+    <hyperlink ref="E80" r:id="rId78" display="https://tenda-api.stoomlab.com.br/api/public/store/product/oleo-de-girassol-soya-900ml-20073"/>
+    <hyperlink ref="E82" r:id="rId79" display="https://tenda-api.stoomlab.com.br/api/public/store/product/papel-higienico-folha-dupla-toque-da-seda-30m-neve-leve-12-pague-11"/>
+    <hyperlink ref="E84" r:id="rId80" display="https://tenda-api.stoomlab.com.br/api/public/store/product/papel-higienico-folha-tripla-neve-20m-leve-24-pague-21-rolos-29414"/>
+    <hyperlink ref="E85" r:id="rId81" display="https://tenda-api.stoomlab.com.br/api/public/store/product/creme-dental-tripla-acao-hortela-colgate-90g"/>
+    <hyperlink ref="F86" r:id="rId82" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891024123560"/>
+    <hyperlink ref="F87" r:id="rId83" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7891024132647"/>
+    <hyperlink ref="E88" r:id="rId84" display="https://tenda-api.stoomlab.com.br/api/public/store/product/creme-dental-sensitive-pro-alivio-colgate-90g-28079"/>
+    <hyperlink ref="E90" r:id="rId85" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-pedra-urca-coco-5-unidades-200g-11265"/>
+    <hyperlink ref="E91" r:id="rId86" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-em-pedra-ype-coco-5x200g-4199"/>
+    <hyperlink ref="E92" r:id="rId87" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-pedra-urca-coco-premium-200g-11296"/>
+    <hyperlink ref="F92" r:id="rId88" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7896056401983"/>
+    <hyperlink ref="E93" r:id="rId89" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sabao-de-pedra-de-coco-ype-200g-27172"/>
+    <hyperlink ref="E94" r:id="rId90" display="https://tenda-api.stoomlab.com.br/api/public/store/product/refil-sabonete-liquido-buque-de-jasmim-lux-220ml-24428"/>
+    <hyperlink ref="E95" r:id="rId91" display="https://tenda-api.stoomlab.com.br/api/public/store/product/refil-sabonete-liquido-flor-de-lotus-lux-200ml-24434"/>
+    <hyperlink ref="E96" r:id="rId92" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sal-refinado-cisne-1kg-304"/>
+    <hyperlink ref="F96" r:id="rId93" display="https://www.jauserve.com.br/on/demandware.store/Sites-JauServe-Site/pt_BR/Product-Show?pid=7896035210001"/>
+    <hyperlink ref="E97" r:id="rId94" display="https://tenda-api.stoomlab.com.br/api/public/store/product/sardinha-em-oleo-gomes-da-costa-125g-525"/>
+    <hyperlink ref="E98" r:id="rId95" display="https://tenda-api.stoomlab.com.br/api/public/store/product/papel-toalha-kitchen-2-unidades-1232"/>
+    <hyperlink ref="E99" r:id="rId96" display="https://tenda-api.stoomlab.com.br/api/public/store/product/toalha-papel-snack-2un-19510"/>
+    <hyperlink ref="E100" r:id="rId97" display="https://tenda-api.stoomlab.com.br/api/public/store/product/papel-toalha-snob-neutro-2-unidades-3291"/>
+    <hyperlink ref="E101" r:id="rId98" display="https://tenda-api.stoomlab.com.br/api/public/store/product/torrada-integral-bauducco-284g-27962"/>
+    <hyperlink ref="E102" r:id="rId99" display="https://tenda-api.stoomlab.com.br/api/public/store/product/vinagre-de-fruta-castelo-maca-750ml-701"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Adding more info in output excel file
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1452,7 +1452,7 @@
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1528,12 +1528,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1614,7 +1608,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1755,10 +1749,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1844,7 +1834,7 @@
       <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -3707,7 +3697,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.14"/>
   </cols>
@@ -3740,7 +3730,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3759,13 +3749,13 @@
   </sheetPr>
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B114" activeCellId="0" sqref="B114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.74"/>
@@ -4418,7 +4408,9 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="28"/>
+      <c r="A35" s="28" t="n">
+        <v>33</v>
+      </c>
       <c r="B35" s="10" t="s">
         <v>60</v>
       </c>
@@ -4435,7 +4427,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>63</v>
@@ -4451,7 +4443,9 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="28"/>
+      <c r="A37" s="28" t="n">
+        <v>35</v>
+      </c>
       <c r="B37" s="10" t="s">
         <v>63</v>
       </c>
@@ -4468,7 +4462,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>235</v>
@@ -4488,7 +4482,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>68</v>
@@ -4508,7 +4502,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>242</v>
@@ -4528,7 +4522,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>73</v>
@@ -4548,7 +4542,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="28" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>74</v>
@@ -4568,7 +4562,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>76</v>
@@ -4588,7 +4582,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>251</v>
@@ -4606,7 +4600,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>79</v>
@@ -4626,7 +4620,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>80</v>
@@ -4646,7 +4640,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>82</v>
@@ -4663,7 +4657,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="28" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>85</v>
@@ -4682,7 +4676,9 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="28"/>
+      <c r="A49" s="28" t="n">
+        <v>47</v>
+      </c>
       <c r="B49" s="4" t="s">
         <v>88</v>
       </c>
@@ -4699,7 +4695,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>88</v>
@@ -4716,7 +4712,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>90</v>
@@ -4733,7 +4729,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="28" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>265</v>
@@ -4753,7 +4749,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>269</v>
@@ -4770,7 +4766,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="28" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>271</v>
@@ -4787,7 +4783,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="28" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>273</v>
@@ -4806,7 +4802,9 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="28"/>
+      <c r="A56" s="28" t="n">
+        <v>54</v>
+      </c>
       <c r="B56" s="4" t="s">
         <v>273</v>
       </c>
@@ -4822,7 +4820,9 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="28"/>
+      <c r="A57" s="28" t="n">
+        <v>55</v>
+      </c>
       <c r="B57" s="4" t="s">
         <v>277</v>
       </c>
@@ -4839,7 +4839,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B58" s="24" t="s">
         <v>279</v>
@@ -4856,7 +4856,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B59" s="24" t="s">
         <v>279</v>
@@ -4876,7 +4876,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>102</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>105</v>
@@ -4916,7 +4916,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>287</v>
@@ -4934,7 +4934,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="n">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>107</v>
@@ -4954,7 +4954,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="n">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>109</v>
@@ -4974,7 +4974,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="n">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>293</v>
@@ -4991,7 +4991,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>295</v>
@@ -5011,7 +5011,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="n">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>298</v>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28" t="n">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>113</v>
@@ -5048,7 +5048,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28" t="n">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>115</v>
@@ -5068,7 +5068,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>304</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="n">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>116</v>
@@ -5108,7 +5108,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>118</v>
@@ -5128,7 +5128,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="n">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>119</v>
@@ -5142,7 +5142,9 @@
       <c r="E73" s="33"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="28"/>
+      <c r="A74" s="28" t="n">
+        <v>72</v>
+      </c>
       <c r="B74" s="4" t="s">
         <v>312</v>
       </c>
@@ -5159,7 +5161,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="n">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>121</v>
@@ -5179,7 +5181,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="n">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B76" s="24" t="s">
         <v>316</v>
@@ -5199,7 +5201,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="n">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B77" s="24" t="s">
         <v>316</v>
@@ -5219,7 +5221,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B78" s="34" t="s">
         <v>321</v>
@@ -5239,7 +5241,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B79" s="24" t="s">
         <v>125</v>
@@ -5259,7 +5261,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B80" s="24" t="s">
         <v>125</v>
@@ -5275,7 +5277,9 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="28"/>
+      <c r="A81" s="28" t="n">
+        <v>79</v>
+      </c>
       <c r="B81" s="24" t="s">
         <v>330</v>
       </c>
@@ -5292,7 +5296,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="n">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>332</v>
@@ -5311,7 +5315,9 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="28"/>
+      <c r="A83" s="28" t="n">
+        <v>81</v>
+      </c>
       <c r="B83" s="4" t="s">
         <v>128</v>
       </c>
@@ -5328,7 +5334,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="n">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>128</v>
@@ -5345,7 +5351,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="n">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>337</v>
@@ -5364,8 +5370,10 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="28"/>
-      <c r="B86" s="35" t="s">
+      <c r="A86" s="28" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>340</v>
       </c>
       <c r="C86" s="5" t="s">
@@ -5380,8 +5388,10 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="28"/>
-      <c r="B87" s="35" t="s">
+      <c r="A87" s="28" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>340</v>
       </c>
       <c r="C87" s="5" t="s">
@@ -5397,7 +5407,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="n">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B88" s="34" t="s">
         <v>345</v>
@@ -5413,7 +5423,9 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="28"/>
+      <c r="A89" s="28" t="n">
+        <v>87</v>
+      </c>
       <c r="B89" s="34" t="s">
         <v>347</v>
       </c>
@@ -5430,7 +5442,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="28" t="n">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B90" s="24" t="s">
         <v>135</v>
@@ -5450,7 +5462,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="28" t="n">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B91" s="24" t="s">
         <v>135</v>
@@ -5470,7 +5482,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="28" t="n">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B92" s="24" t="s">
         <v>135</v>
@@ -5490,7 +5502,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="28" t="n">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B93" s="24" t="s">
         <v>135</v>
@@ -5507,7 +5519,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="28" t="n">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>138</v>
@@ -5524,7 +5536,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="28" t="n">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>140</v>
@@ -5541,7 +5553,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="28" t="n">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>359</v>
@@ -5561,7 +5573,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="28" t="n">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>143</v>
@@ -5581,7 +5593,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="n">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B98" s="24" t="s">
         <v>145</v>
@@ -5601,7 +5613,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="28" t="n">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B99" s="24" t="s">
         <v>145</v>
@@ -5618,7 +5630,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="28" t="n">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B100" s="24" t="s">
         <v>145</v>
@@ -5638,7 +5650,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="28" t="n">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>150</v>
@@ -5658,7 +5670,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="28" t="n">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>153</v>

</xml_diff>